<commit_message>
modif taille d'une main et modif répartition
</commit_message>
<xml_diff>
--- a/D-specs.xlsx
+++ b/D-specs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gab\Documents\Polytech\SI3\ps5\dojo-poker-2021-poker-2021-d\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09039D45-B5A8-49BC-B998-4C633A63AE57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B99BF7-7A9B-4758-9D9E-10DD59DADE9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -637,7 +637,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -870,7 +870,7 @@
         <v>34</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="D10" t="s">
         <v>18</v>
@@ -894,7 +894,7 @@
         <v>35</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="D11" t="s">
         <v>25</v>

</xml_diff>